<commit_message>
Ajout du README du TD1
</commit_message>
<xml_diff>
--- a/assets/module1/network_informations.xlsx
+++ b/assets/module1/network_informations.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>HQ</t>
   </si>
@@ -65,15 +65,65 @@
   </si>
   <si>
     <t>se0/</t>
+  </si>
+  <si>
+    <t>Branch3</t>
+  </si>
+  <si>
+    <t>Adresse réseau</t>
+  </si>
+  <si>
+    <t>Masque de sous-réseau décimal</t>
+  </si>
+  <si>
+    <t>Masque de sous-réseau CIDR</t>
+  </si>
+  <si>
+    <t>Première adresse IP utilisable</t>
+  </si>
+  <si>
+    <t>Dernière adresse IP utilisable</t>
+  </si>
+  <si>
+    <t>Adresse de diffusion</t>
+  </si>
+  <si>
+    <t>Routeur</t>
+  </si>
+  <si>
+    <t>Adresse réseau de destination</t>
+  </si>
+  <si>
+    <t>Masque de réseau</t>
+  </si>
+  <si>
+    <t>Passerelle</t>
+  </si>
+  <si>
+    <t>Table de routage statique</t>
+  </si>
+  <si>
+    <t>Table d'addressage des interfaces</t>
+  </si>
+  <si>
+    <t>Table d'addressage des sous réseaux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,6 +168,48 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:G23" totalsRowShown="0">
+  <autoFilter ref="B3:G23"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Adresse réseau"/>
+    <tableColumn id="2" name="Masque de sous-réseau décimal"/>
+    <tableColumn id="3" name="Masque de sous-réseau CIDR"/>
+    <tableColumn id="4" name="Première adresse IP utilisable"/>
+    <tableColumn id="5" name="Dernière adresse IP utilisable"/>
+    <tableColumn id="6" name="Adresse de diffusion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:F15" totalsRowShown="0">
+  <autoFilter ref="B3:F15"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Périphérique"/>
+    <tableColumn id="2" name=" Interface"/>
+    <tableColumn id="3" name=" Adresse IP"/>
+    <tableColumn id="4" name=" Masque de sous-réseau"/>
+    <tableColumn id="5" name=" Passerelle par défaut"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B3:E26" totalsRowShown="0">
+  <autoFilter ref="B3:E26"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Routeur"/>
+    <tableColumn id="2" name="Adresse réseau de destination"/>
+    <tableColumn id="3" name="Masque de réseau"/>
+    <tableColumn id="4" name="Passerelle"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,163 +475,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="B1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifiction du tableau Excel
</commit_message>
<xml_diff>
--- a/assets/module1/network_informations.xlsx
+++ b/assets/module1/network_informations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="networks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>HQ</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Branch3</t>
   </si>
   <si>
-    <t>Adresse réseau</t>
-  </si>
-  <si>
     <t>Masque de sous-réseau décimal</t>
   </si>
   <si>
@@ -107,6 +104,177 @@
   </si>
   <si>
     <t>Table d'addressage des sous réseaux</t>
+  </si>
+  <si>
+    <t>Adresse de sous réseau</t>
+  </si>
+  <si>
+    <t>192.168.1.0</t>
+  </si>
+  <si>
+    <t>/26</t>
+  </si>
+  <si>
+    <t>255.255.255.192</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>192.168.1.62</t>
+  </si>
+  <si>
+    <t>192.168.1.63</t>
+  </si>
+  <si>
+    <t>Sous réseaux</t>
+  </si>
+  <si>
+    <t>LAN1-HQ</t>
+  </si>
+  <si>
+    <t>/27</t>
+  </si>
+  <si>
+    <t>/28</t>
+  </si>
+  <si>
+    <t>/30</t>
+  </si>
+  <si>
+    <t>LAN2-HQ</t>
+  </si>
+  <si>
+    <t>LAN1-BRANCH1</t>
+  </si>
+  <si>
+    <t>LAN1-BRANCH2</t>
+  </si>
+  <si>
+    <t>LAN2-BRANCH2</t>
+  </si>
+  <si>
+    <t>LAN2-BRANCH1</t>
+  </si>
+  <si>
+    <t>WAN-HQ-BRANCH1</t>
+  </si>
+  <si>
+    <t>WAN-HQ-BRANCH2</t>
+  </si>
+  <si>
+    <t>WAN-BRANCH1-BRANCH2</t>
+  </si>
+  <si>
+    <t>192.168.1.64</t>
+  </si>
+  <si>
+    <t>192.168.1.65</t>
+  </si>
+  <si>
+    <t>192.168.1.126</t>
+  </si>
+  <si>
+    <t>192.168.1.127</t>
+  </si>
+  <si>
+    <t>192.168.1.128</t>
+  </si>
+  <si>
+    <t>192.168.1.129</t>
+  </si>
+  <si>
+    <t>192.168.1.158</t>
+  </si>
+  <si>
+    <t>255.255.255.224</t>
+  </si>
+  <si>
+    <t>192.168.1.159</t>
+  </si>
+  <si>
+    <t>192.168.1.160</t>
+  </si>
+  <si>
+    <t>192.168.1.161</t>
+  </si>
+  <si>
+    <t>192.168.1.190</t>
+  </si>
+  <si>
+    <t>192.168.1.191</t>
+  </si>
+  <si>
+    <t>192.168.1.192</t>
+  </si>
+  <si>
+    <t>255.255.255.240</t>
+  </si>
+  <si>
+    <t>192.168.1.193</t>
+  </si>
+  <si>
+    <t>192.168.1.223</t>
+  </si>
+  <si>
+    <t>192.168.1.222</t>
+  </si>
+  <si>
+    <t>192.168.1.224</t>
+  </si>
+  <si>
+    <t>192.168.1.208</t>
+  </si>
+  <si>
+    <t>192.168.1.207</t>
+  </si>
+  <si>
+    <t>192.168.1.206</t>
+  </si>
+  <si>
+    <t>192.168.1.209</t>
+  </si>
+  <si>
+    <t>255.255.255.252</t>
+  </si>
+  <si>
+    <t>192.168.1.225</t>
+  </si>
+  <si>
+    <t>192.168.1.226</t>
+  </si>
+  <si>
+    <t>192.168.1.227</t>
+  </si>
+  <si>
+    <t>192.168.1.228</t>
+  </si>
+  <si>
+    <t>255.255.255.253</t>
+  </si>
+  <si>
+    <t>255.255.255.254</t>
+  </si>
+  <si>
+    <t>192.168.1.229</t>
+  </si>
+  <si>
+    <t>192.168.1.230</t>
+  </si>
+  <si>
+    <t>192.168.1.231</t>
+  </si>
+  <si>
+    <t>192.168.1.232</t>
+  </si>
+  <si>
+    <t>192.168.1.233</t>
+  </si>
+  <si>
+    <t>192.168.1.234</t>
+  </si>
+  <si>
+    <t>192.168.1.235</t>
   </si>
 </sst>
 </file>
@@ -130,15 +298,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,13 +320,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,10 +359,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:G23" totalsRowShown="0">
-  <autoFilter ref="B3:G23"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Adresse réseau"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:H23" totalsRowShown="0">
+  <autoFilter ref="B3:H23"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Sous réseaux"/>
+    <tableColumn id="7" name="Adresse de sous réseau"/>
     <tableColumn id="2" name="Masque de sous-réseau décimal"/>
     <tableColumn id="3" name="Masque de sous-réseau CIDR"/>
     <tableColumn id="4" name="Première adresse IP utilisable"/>
@@ -475,46 +664,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G3"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.21875" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:8" ht="46.2" x14ac:dyDescent="0.85">
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -528,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -542,7 +946,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="46.2" x14ac:dyDescent="0.85">
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -706,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -718,21 +1122,21 @@
   <sheetData>
     <row r="1" spans="2:5" ht="46.2" x14ac:dyDescent="0.85">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>